<commit_message>
food-details 코드 오류 해결
</commit_message>
<xml_diff>
--- a/data/group_test_ㅇㅇ_2024-01-30.xlsx
+++ b/data/group_test_ㅇㅇ_2024-01-30.xlsx
@@ -1580,14 +1580,180 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Food Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Food Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Ingredient Code</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ingrdient</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>1 person (g)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Caramelized Pork with Eggs</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>H0002</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Pork meat, lean, raw</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Caramelized Pork with Eggs</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>B0008</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Garlic, fresh, raw</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>6.66</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Caramelized Pork with Eggs</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>N0001</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Salt, table</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Num Banchok</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>N0005</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Noodle, rice flour, wet</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Num Banchok</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>J0012</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Fish, Mystus wolffi, raw</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Num Banchok</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>G0001</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sugar, granulated</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>